<commit_message>
changed rowStart to columnStart mistake
</commit_message>
<xml_diff>
--- a/SpreadCheck/Test WorkBook.xlsx
+++ b/SpreadCheck/Test WorkBook.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah Rawlinson\Documents\GitHub\RPG Course 2nd Start\SpreadCheck\SpreadCheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D52F991-1C29-4091-B5E3-E4332757BCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43E81CF-D77A-45FB-A01E-6E111D7BAA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D8B4C602-9FBB-485D-8012-D731F932D843}"/>
+    <workbookView xWindow="59025" yWindow="13410" windowWidth="14400" windowHeight="7665" activeTab="1" xr2:uid="{D8B4C602-9FBB-485D-8012-D731F932D843}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Errors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
   <si>
     <t>Warn If Error Test</t>
   </si>
@@ -70,6 +71,39 @@
   </si>
   <si>
     <t>/// &amp;&amp;</t>
+  </si>
+  <si>
+    <t>COLUMN</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Recieved</t>
+  </si>
+  <si>
+    <t>Cell Contains a Space</t>
+  </si>
+  <si>
+    <t>No Spaces</t>
+  </si>
+  <si>
+    <t>Cell Contains Non-AlphaNumerics</t>
+  </si>
+  <si>
+    <t>A-Z / 0-9</t>
+  </si>
+  <si>
+    <t>Cell Contains Letters</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -85,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008B8B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,8 +145,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346B9E24-B970-4489-BD73-E654097C239F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -496,4 +537,321 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4859D67D-57CB-483D-AB09-35FC8F537060}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>5555</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>5555</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <v>5555</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>5555</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>5555</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>5555</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>5555</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9">
+        <v>5555</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed last row from column rules to last column variable in form1
</commit_message>
<xml_diff>
--- a/SpreadCheck/Test WorkBook.xlsx
+++ b/SpreadCheck/Test WorkBook.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah Rawlinson\Documents\GitHub\RPG Course 2nd Start\SpreadCheck\SpreadCheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43E81CF-D77A-45FB-A01E-6E111D7BAA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DA820-941E-447B-A8BD-91DC792AB333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59025" yWindow="13410" windowWidth="14400" windowHeight="7665" activeTab="1" xr2:uid="{D8B4C602-9FBB-485D-8012-D731F932D843}"/>
+    <workbookView xWindow="57480" yWindow="11880" windowWidth="29040" windowHeight="15840" xr2:uid="{D8B4C602-9FBB-485D-8012-D731F932D843}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Errors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Warn If Error Test</t>
   </si>
@@ -71,39 +70,6 @@
   </si>
   <si>
     <t>/// &amp;&amp;</t>
-  </si>
-  <si>
-    <t>COLUMN</t>
-  </si>
-  <si>
-    <t>ROW</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>Recieved</t>
-  </si>
-  <si>
-    <t>Cell Contains a Space</t>
-  </si>
-  <si>
-    <t>No Spaces</t>
-  </si>
-  <si>
-    <t>Cell Contains Non-AlphaNumerics</t>
-  </si>
-  <si>
-    <t>A-Z / 0-9</t>
-  </si>
-  <si>
-    <t>Cell Contains Letters</t>
-  </si>
-  <si>
-    <t>String</t>
   </si>
 </sst>
 </file>
@@ -119,18 +85,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008B8B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,9 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346B9E24-B970-4489-BD73-E654097C239F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,321 +493,152 @@
         <v>55555</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4859D67D-57CB-483D-AB09-35FC8F537060}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>5555</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="b">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5555</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="b">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>5555</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5555</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="b">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>5555</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>5555</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="J2">
-        <v>5555</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="E10">
+        <v>5555</v>
+      </c>
+      <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3">
-        <v>5555</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <v>5555</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>5555</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>5555</v>
-      </c>
-      <c r="K6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7">
-        <v>5555</v>
-      </c>
-      <c r="K7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8">
-        <v>5555</v>
-      </c>
-      <c r="K8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9">
-        <v>5555</v>
-      </c>
-      <c r="K9" t="s">
-        <v>10</v>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>5555</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>55555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>